<commit_message>
fix: fixed output csv formmatting
</commit_message>
<xml_diff>
--- a/Model_Comparation (version 1).xlsb.xlsx
+++ b/Model_Comparation (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfria\Projects\ironhacks\PROJECT_Natural_Language_Processing_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EB6EBDE-6E95-4905-9D17-F7052DD8C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE5C7C1-E2A0-4555-8AF0-FA93C3C7292D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Stemming</t>
   </si>
@@ -47,6 +46,15 @@
   </si>
   <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t>wor2vec (svm)</t>
+  </si>
+  <si>
+    <t>GloVe (logistic regresion)</t>
+  </si>
+  <si>
+    <t>Glove (random forest</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,6 +1570,30 @@
       </c>
       <c r="C6">
         <v>0.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>